<commit_message>
Modified and Annotated image 261 - 328
</commit_message>
<xml_diff>
--- a/Error_Annotations.xlsx
+++ b/Error_Annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spectroGUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6928BEC6-6859-4EF0-8D22-9EB2F7ACF1CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3657F3F-C503-4A11-981D-ABB031843B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
   <si>
     <t>Picture Number</t>
   </si>
@@ -184,10 +184,19 @@
     </r>
   </si>
   <si>
-    <t>Alcohol, Aromatic</t>
-  </si>
-  <si>
     <t>Amine, Alcohol</t>
+  </si>
+  <si>
+    <t>Broken image (No visible aromatic signals around 700 - 900)</t>
+  </si>
+  <si>
+    <t>Aromatic, Unknown</t>
+  </si>
+  <si>
+    <t>Wide, strong preak at 3200 - 2300; no visible C=O at 1725 - 1700</t>
+  </si>
+  <si>
+    <t>Aromatic, Alcohol</t>
   </si>
 </sst>
 </file>
@@ -529,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -629,77 +638,77 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="2">
+        <v>84</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>103</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>134</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>135</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
+      <c r="A11" s="2">
+        <v>113</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -712,98 +721,98 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" s="2">
-        <v>153</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>20</v>
+      <c r="A13">
+        <v>135</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" s="2">
-        <v>156</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>23</v>
+      <c r="A14">
+        <v>145</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
-        <v>207</v>
+        <v>159</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
-        <v>208</v>
+        <v>175</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>20</v>
@@ -811,35 +820,35 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>18</v>
@@ -848,12 +857,12 @@
         <v>27</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>18</v>
@@ -862,35 +871,119 @@
         <v>27</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
+        <v>215</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" s="2">
+        <v>221</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" s="2">
         <v>224</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" s="2">
+        <v>272</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>316</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>16</v>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>317</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" s="2">
+        <v>322</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified and annotated image 260 - 370. Removed all Aromatic bounding boxes at 1600.
</commit_message>
<xml_diff>
--- a/Error_Annotations.xlsx
+++ b/Error_Annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spectroGUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3657F3F-C503-4A11-981D-ABB031843B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2F3F33-06E5-4756-8C91-E468B37307F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="46">
   <si>
     <t>Picture Number</t>
   </si>
@@ -197,6 +197,18 @@
   </si>
   <si>
     <t>Aromatic, Alcohol</t>
+  </si>
+  <si>
+    <t>Image not in the right resolution</t>
+  </si>
+  <si>
+    <t>Aromatic, Alcohol, Phenol</t>
+  </si>
+  <si>
+    <t>No wide, strong peak at 3600 - 3100</t>
+  </si>
+  <si>
+    <t>Alkene, Ketone, Alcohol</t>
   </si>
 </sst>
 </file>
@@ -538,16 +550,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.53125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.9296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="61.46484375" bestFit="1" customWidth="1"/>
   </cols>
@@ -581,16 +593,16 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="3">
+      <c r="A3">
         <v>37</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -948,13 +960,13 @@
       <c r="A29">
         <v>316</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
         <v>38</v>
       </c>
     </row>
@@ -962,13 +974,13 @@
       <c r="A30">
         <v>317</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="3" t="s">
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
         <v>38</v>
       </c>
     </row>
@@ -984,6 +996,188 @@
       </c>
       <c r="D31" s="2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>333</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" s="2">
+        <v>336</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" s="2">
+        <v>337</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A35" s="2">
+        <v>339</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36" s="2">
+        <v>340</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" s="2">
+        <v>341</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A38" s="2">
+        <v>343</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A39" s="2">
+        <v>346</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A40" s="2">
+        <v>347</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A41" s="2">
+        <v>348</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A42" s="2">
+        <v>352</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A43" s="3">
+        <v>358</v>
+      </c>
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A44" s="3">
+        <v>364</v>
+      </c>
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified and annotated image 370 - 670.
</commit_message>
<xml_diff>
--- a/Error_Annotations.xlsx
+++ b/Error_Annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spectroGUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2F3F33-06E5-4756-8C91-E468B37307F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC12CE6-52A8-4407-BAB9-55A4372B36FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="70">
   <si>
     <t>Picture Number</t>
   </si>
@@ -209,6 +209,101 @@
   </si>
   <si>
     <t>Alkene, Ketone, Alcohol</t>
+  </si>
+  <si>
+    <t>Ketone</t>
+  </si>
+  <si>
+    <t>Narrow, strong peak at 1680 - 1600</t>
+  </si>
+  <si>
+    <t>Alcohol, Alkyne</t>
+  </si>
+  <si>
+    <t>Alcohol, Symmetrical Alkyne</t>
+  </si>
+  <si>
+    <t>Alkene, Amide</t>
+  </si>
+  <si>
+    <t>Esters</t>
+  </si>
+  <si>
+    <t>Ester, Nitrile</t>
+  </si>
+  <si>
+    <t>Narrow, strong peak at 2150</t>
+  </si>
+  <si>
+    <t>Narrow, strong peak at 1680 - 1650</t>
+  </si>
+  <si>
+    <t>Amine, Ketone</t>
+  </si>
+  <si>
+    <t>Narrow, strong peaks at 2200, 2100; Narrow, moderate peaks at 3400 - 3300</t>
+  </si>
+  <si>
+    <t>Amine, Nitrile, Aromatic</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>No aromatic peak at 900 - 700</t>
+  </si>
+  <si>
+    <t>Alcohol, Amine</t>
+  </si>
+  <si>
+    <t>Alcohol, Amine, Alkene</t>
+  </si>
+  <si>
+    <t>Alcohol, Tertiary Amine, Alkene</t>
+  </si>
+  <si>
+    <t>Ketone, Alkene</t>
+  </si>
+  <si>
+    <t>Alcohol, Alkene, Carboxylic Acids</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Alcohol, Symmertical / </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Trans</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Alkene</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcohol, Aldehyde, Amine</t>
+  </si>
+  <si>
+    <t>Alcohol, Aldehyde</t>
+  </si>
+  <si>
+    <t>Alcohol, Amine, Carboxylic Acids</t>
+  </si>
+  <si>
+    <t>Alcohol, Tertiary Amine, Carboxylic Acid</t>
   </si>
 </sst>
 </file>
@@ -550,17 +645,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.53125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="61.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1008,7 +1103,7 @@
       <c r="C32" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1153,7 +1248,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A43" s="3">
+      <c r="A43">
         <v>358</v>
       </c>
       <c r="B43" t="s">
@@ -1167,7 +1262,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A44" s="3">
+      <c r="A44">
         <v>364</v>
       </c>
       <c r="B44" t="s">
@@ -1178,6 +1273,580 @@
       </c>
       <c r="D44" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>372</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>39</v>
+      </c>
+      <c r="D45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>382</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>383</v>
+      </c>
+      <c r="B47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>389</v>
+      </c>
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>405</v>
+      </c>
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>424</v>
+      </c>
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>433</v>
+      </c>
+      <c r="B51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" t="s">
+        <v>50</v>
+      </c>
+      <c r="D51" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>436</v>
+      </c>
+      <c r="B52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>443</v>
+      </c>
+      <c r="B53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>446</v>
+      </c>
+      <c r="B54" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" t="s">
+        <v>50</v>
+      </c>
+      <c r="D54" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>447</v>
+      </c>
+      <c r="B55" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>453</v>
+      </c>
+      <c r="B56" t="s">
+        <v>51</v>
+      </c>
+      <c r="C56" t="s">
+        <v>52</v>
+      </c>
+      <c r="D56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>457</v>
+      </c>
+      <c r="B57" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>459</v>
+      </c>
+      <c r="B58" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58" t="s">
+        <v>27</v>
+      </c>
+      <c r="D58" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>460</v>
+      </c>
+      <c r="B59" t="s">
+        <v>55</v>
+      </c>
+      <c r="C59" t="s">
+        <v>55</v>
+      </c>
+      <c r="D59" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>467</v>
+      </c>
+      <c r="B60" t="s">
+        <v>21</v>
+      </c>
+      <c r="C60" t="s">
+        <v>22</v>
+      </c>
+      <c r="D60" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>469</v>
+      </c>
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>57</v>
+      </c>
+      <c r="D61" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>470</v>
+      </c>
+      <c r="B62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s">
+        <v>58</v>
+      </c>
+      <c r="D62" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>471</v>
+      </c>
+      <c r="B63" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" t="s">
+        <v>35</v>
+      </c>
+      <c r="D63" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>482</v>
+      </c>
+      <c r="B64" t="s">
+        <v>60</v>
+      </c>
+      <c r="C64" t="s">
+        <v>60</v>
+      </c>
+      <c r="D64" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>486</v>
+      </c>
+      <c r="B65" t="s">
+        <v>61</v>
+      </c>
+      <c r="C65" t="s">
+        <v>62</v>
+      </c>
+      <c r="D65" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A66">
+        <v>487</v>
+      </c>
+      <c r="B66" t="s">
+        <v>46</v>
+      </c>
+      <c r="C66" t="s">
+        <v>63</v>
+      </c>
+      <c r="D66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A67">
+        <v>495</v>
+      </c>
+      <c r="B67" t="s">
+        <v>64</v>
+      </c>
+      <c r="C67" t="s">
+        <v>64</v>
+      </c>
+      <c r="D67" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A68">
+        <v>497</v>
+      </c>
+      <c r="B68" t="s">
+        <v>33</v>
+      </c>
+      <c r="C68" t="s">
+        <v>34</v>
+      </c>
+      <c r="D68" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A69">
+        <v>510</v>
+      </c>
+      <c r="B69" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" t="s">
+        <v>31</v>
+      </c>
+      <c r="D69" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A70">
+        <v>533</v>
+      </c>
+      <c r="B70" t="s">
+        <v>21</v>
+      </c>
+      <c r="C70" t="s">
+        <v>65</v>
+      </c>
+      <c r="D70" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A71">
+        <v>553</v>
+      </c>
+      <c r="B71" t="s">
+        <v>21</v>
+      </c>
+      <c r="C71" t="s">
+        <v>22</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A72">
+        <v>559</v>
+      </c>
+      <c r="B72" t="s">
+        <v>18</v>
+      </c>
+      <c r="C72" t="s">
+        <v>27</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A73">
+        <v>562</v>
+      </c>
+      <c r="B73" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A74">
+        <v>563</v>
+      </c>
+      <c r="B74" t="s">
+        <v>18</v>
+      </c>
+      <c r="C74" t="s">
+        <v>27</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A75">
+        <v>564</v>
+      </c>
+      <c r="B75" t="s">
+        <v>18</v>
+      </c>
+      <c r="C75" t="s">
+        <v>27</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A76">
+        <v>573</v>
+      </c>
+      <c r="B76" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" t="s">
+        <v>27</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A77">
+        <v>580</v>
+      </c>
+      <c r="B77" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" t="s">
+        <v>31</v>
+      </c>
+      <c r="D77" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A78">
+        <v>616</v>
+      </c>
+      <c r="B78" t="s">
+        <v>67</v>
+      </c>
+      <c r="C78" t="s">
+        <v>66</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A79">
+        <v>651</v>
+      </c>
+      <c r="B79" t="s">
+        <v>18</v>
+      </c>
+      <c r="C79" t="s">
+        <v>19</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A80">
+        <v>652</v>
+      </c>
+      <c r="B80" t="s">
+        <v>68</v>
+      </c>
+      <c r="C80" t="s">
+        <v>69</v>
+      </c>
+      <c r="D80" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A81">
+        <v>654</v>
+      </c>
+      <c r="B81" t="s">
+        <v>68</v>
+      </c>
+      <c r="C81" t="s">
+        <v>69</v>
+      </c>
+      <c r="D81" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A82">
+        <v>655</v>
+      </c>
+      <c r="B82" t="s">
+        <v>18</v>
+      </c>
+      <c r="C82" t="s">
+        <v>27</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A83">
+        <v>660</v>
+      </c>
+      <c r="B83" t="s">
+        <v>18</v>
+      </c>
+      <c r="C83" t="s">
+        <v>19</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A84">
+        <v>661</v>
+      </c>
+      <c r="B84" t="s">
+        <v>68</v>
+      </c>
+      <c r="C84" t="s">
+        <v>69</v>
+      </c>
+      <c r="D84" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A85">
+        <v>666</v>
+      </c>
+      <c r="B85" t="s">
+        <v>18</v>
+      </c>
+      <c r="C85" t="s">
+        <v>19</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified and Annotated image 670 - 1000
</commit_message>
<xml_diff>
--- a/Error_Annotations.xlsx
+++ b/Error_Annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spectroGUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC12CE6-52A8-4407-BAB9-55A4372B36FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178DEF00-58DB-4866-AA38-06FD30769D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="101">
   <si>
     <t>Picture Number</t>
   </si>
@@ -268,8 +268,23 @@
     <t>Alcohol, Alkene, Carboxylic Acids</t>
   </si>
   <si>
+    <t>Alcohol, Aldehyde, Amine</t>
+  </si>
+  <si>
+    <t>Alcohol, Aldehyde</t>
+  </si>
+  <si>
+    <t>Alcohol, Amine, Carboxylic Acids</t>
+  </si>
+  <si>
+    <t>Alcohol, Tertiary Amine, Carboxylic Acid</t>
+  </si>
+  <si>
+    <t>Nitrile, Alkene</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Alcohol, Symmertical / </t>
+      <t xml:space="preserve">Alcohol, Symmertrical / </t>
     </r>
     <r>
       <rPr>
@@ -294,23 +309,124 @@
     </r>
   </si>
   <si>
-    <t>Alcohol, Aldehyde, Amine</t>
-  </si>
-  <si>
-    <t>Alcohol, Aldehyde</t>
-  </si>
-  <si>
-    <t>Alcohol, Amine, Carboxylic Acids</t>
-  </si>
-  <si>
-    <t>Alcohol, Tertiary Amine, Carboxylic Acid</t>
+    <r>
+      <t xml:space="preserve">Nitrile, Symmertrical / </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Trans</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Alkene</t>
+    </r>
+  </si>
+  <si>
+    <t>Alkene, Ester</t>
+  </si>
+  <si>
+    <t>Narrow, strong peak at 1750 - 1730</t>
+  </si>
+  <si>
+    <t>Narrow, strong peak at 3300 - 3100</t>
+  </si>
+  <si>
+    <t>Nitrile</t>
+  </si>
+  <si>
+    <t>Nitrile, Amide</t>
+  </si>
+  <si>
+    <t>Nirtile, Alkene</t>
+  </si>
+  <si>
+    <t>Nitrile, Alkene, Amide</t>
+  </si>
+  <si>
+    <t>Narrow, strong peak at 3400, 3300, 3100</t>
+  </si>
+  <si>
+    <t>Aromatic, Alcohol, Phenol, Amine</t>
+  </si>
+  <si>
+    <t>Aromatic, Ketone</t>
+  </si>
+  <si>
+    <t>Aromatic, Ketone, Amine</t>
+  </si>
+  <si>
+    <t>Narrow, strong peak at 3400, 3200</t>
+  </si>
+  <si>
+    <t>Aromatic, Amine, Amide</t>
+  </si>
+  <si>
+    <t>Narrow, strong peak at 1680</t>
+  </si>
+  <si>
+    <t>No wide, strong peak at 3600 - 3100; Narrow strong peak at 3400, 3300</t>
+  </si>
+  <si>
+    <t>Alkene, Alcohol</t>
+  </si>
+  <si>
+    <t>Aromatic, Amide</t>
+  </si>
+  <si>
+    <t>Narrow, strong peak at 1680; Narrow strong peak at 3400, 3100</t>
+  </si>
+  <si>
+    <t>Aromatic, Alcohol, Phenol, Ketone</t>
+  </si>
+  <si>
+    <t>Narrow, strong peak at 1700</t>
+  </si>
+  <si>
+    <t>Aromatic, Alcohol, Carboxylic Acid</t>
+  </si>
+  <si>
+    <t>No narrow, strong peak at 1720</t>
+  </si>
+  <si>
+    <t>Aromatic, Carboxylic Acid</t>
+  </si>
+  <si>
+    <t>No wide, strong peak at 3600 - 3101</t>
+  </si>
+  <si>
+    <t>Alkene, Aldehyde</t>
+  </si>
+  <si>
+    <t>Alkene, Aldehyde, Alcohol</t>
+  </si>
+  <si>
+    <t>Ketone, Alcohol</t>
+  </si>
+  <si>
+    <t>No narrow, strong peak at 1650</t>
+  </si>
+  <si>
+    <t>No narrow, strong peak at 1700</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,19 +449,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -360,11 +476,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,16 +759,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B151" sqref="B151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.46484375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="61.46484375" bestFit="1" customWidth="1"/>
   </cols>
@@ -674,16 +788,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -702,16 +816,16 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="2">
+      <c r="A4">
         <v>45</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -730,58 +844,58 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="2">
+      <c r="A6">
         <v>71</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="2">
+      <c r="A7">
         <v>83</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="2">
+      <c r="A8">
         <v>84</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="2">
+      <c r="A9">
         <v>85</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>40</v>
       </c>
     </row>
@@ -800,16 +914,16 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" s="2">
+      <c r="A11">
         <v>113</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -856,198 +970,198 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" s="2">
+      <c r="A15">
         <v>153</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" s="2">
+      <c r="A16">
         <v>156</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" s="2">
+      <c r="A17">
         <v>157</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" s="2">
+      <c r="A18">
         <v>159</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="2">
+      <c r="A19">
         <v>175</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="2">
+      <c r="A20">
         <v>207</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" s="2">
+      <c r="A21">
         <v>208</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="2">
+      <c r="A22">
         <v>209</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" s="2">
+      <c r="A23">
         <v>210</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24" s="2">
+      <c r="A24">
         <v>212</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" s="2">
+      <c r="A25">
         <v>215</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" s="2">
+      <c r="A26">
         <v>221</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" s="2">
+      <c r="A27">
         <v>224</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A28" s="2">
+      <c r="A28">
         <v>272</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1080,16 +1194,16 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A31" s="2">
+      <c r="A31">
         <v>322</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1108,142 +1222,142 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A33" s="2">
+      <c r="A33">
         <v>336</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A34" s="2">
+      <c r="A34">
         <v>337</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A35" s="2">
+      <c r="A35">
         <v>339</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A36" s="2">
+      <c r="A36">
         <v>340</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A37" s="2">
+      <c r="A37">
         <v>341</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A38" s="2">
+      <c r="A38">
         <v>343</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="2" t="s">
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A39" s="2">
+      <c r="A39">
         <v>346</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A40" s="2">
+      <c r="A40">
         <v>347</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="2" t="s">
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
         <v>41</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A41" s="2">
+      <c r="A41">
         <v>348</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A42" s="2">
+      <c r="A42">
         <v>352</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1613,77 +1727,77 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69">
-        <v>510</v>
+        <v>533</v>
       </c>
       <c r="B69" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C69" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="D69" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70">
-        <v>533</v>
+        <v>553</v>
       </c>
       <c r="B70" t="s">
         <v>21</v>
       </c>
       <c r="C70" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="D70" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71">
-        <v>553</v>
+        <v>559</v>
       </c>
       <c r="B71" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C71" t="s">
-        <v>22</v>
-      </c>
-      <c r="D71" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D71" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B72" t="s">
         <v>18</v>
       </c>
       <c r="C72" t="s">
-        <v>27</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="D72" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B73" t="s">
         <v>18</v>
       </c>
       <c r="C73" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D73" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B74" t="s">
         <v>18</v>
@@ -1691,13 +1805,13 @@
       <c r="C74" t="s">
         <v>27</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="D74" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75">
-        <v>564</v>
+        <v>573</v>
       </c>
       <c r="B75" t="s">
         <v>18</v>
@@ -1705,75 +1819,75 @@
       <c r="C75" t="s">
         <v>27</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="D75" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76">
-        <v>573</v>
+        <v>580</v>
       </c>
       <c r="B76" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>27</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="D76" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77">
-        <v>580</v>
+        <v>616</v>
       </c>
       <c r="B77" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="C77" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="D77" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78">
-        <v>616</v>
+        <v>651</v>
       </c>
       <c r="B78" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="C78" t="s">
-        <v>66</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="D78" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B79" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="C79" t="s">
-        <v>19</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>20</v>
+        <v>68</v>
+      </c>
+      <c r="D79" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="B80" t="s">
+        <v>67</v>
+      </c>
+      <c r="C80" t="s">
         <v>68</v>
-      </c>
-      <c r="C80" t="s">
-        <v>69</v>
       </c>
       <c r="D80" t="s">
         <v>32</v>
@@ -1781,63 +1895,63 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B81" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="C81" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="D81" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="B82" t="s">
         <v>18</v>
       </c>
       <c r="C82" t="s">
-        <v>27</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="D82" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B83" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="C83" t="s">
-        <v>19</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>20</v>
+        <v>68</v>
+      </c>
+      <c r="D83" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84">
-        <v>661</v>
+        <v>666</v>
       </c>
       <c r="B84" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="C84" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="D84" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85">
-        <v>666</v>
+        <v>708</v>
       </c>
       <c r="B85" t="s">
         <v>18</v>
@@ -1845,11 +1959,880 @@
       <c r="C85" t="s">
         <v>19</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="D85" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A86">
+        <v>711</v>
+      </c>
+      <c r="B86" t="s">
+        <v>69</v>
+      </c>
+      <c r="C86" t="s">
+        <v>71</v>
+      </c>
+      <c r="D86" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A87">
+        <v>729</v>
+      </c>
+      <c r="B87" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87" t="s">
+        <v>72</v>
+      </c>
+      <c r="D87" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A88">
+        <v>730</v>
+      </c>
+      <c r="B88" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" t="s">
+        <v>72</v>
+      </c>
+      <c r="D88" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A89">
+        <v>736</v>
+      </c>
+      <c r="B89" t="s">
+        <v>6</v>
+      </c>
+      <c r="C89" t="s">
+        <v>37</v>
+      </c>
+      <c r="D89" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A90">
+        <v>739</v>
+      </c>
+      <c r="B90" t="s">
+        <v>75</v>
+      </c>
+      <c r="C90" t="s">
+        <v>76</v>
+      </c>
+      <c r="D90" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A91">
+        <v>750</v>
+      </c>
+      <c r="B91" t="s">
+        <v>77</v>
+      </c>
+      <c r="C91" t="s">
+        <v>71</v>
+      </c>
+      <c r="D91" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A92">
+        <v>751</v>
+      </c>
+      <c r="B92" t="s">
+        <v>77</v>
+      </c>
+      <c r="C92" t="s">
+        <v>78</v>
+      </c>
+      <c r="D92" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A93">
+        <v>785</v>
+      </c>
+      <c r="B93" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A94">
+        <v>786</v>
+      </c>
+      <c r="B94" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A95">
+        <v>788</v>
+      </c>
+      <c r="B95" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95" t="s">
+        <v>7</v>
+      </c>
+      <c r="D95" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A96">
+        <v>789</v>
+      </c>
+      <c r="B96" t="s">
+        <v>7</v>
+      </c>
+      <c r="C96" t="s">
+        <v>7</v>
+      </c>
+      <c r="D96" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A97">
+        <v>801</v>
+      </c>
+      <c r="B97" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A98">
+        <v>802</v>
+      </c>
+      <c r="B98" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" t="s">
+        <v>5</v>
+      </c>
+      <c r="D98" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A99">
+        <v>803</v>
+      </c>
+      <c r="B99" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99" t="s">
+        <v>41</v>
+      </c>
+      <c r="D99" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A100">
+        <v>804</v>
+      </c>
+      <c r="B100" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A101">
+        <v>811</v>
+      </c>
+      <c r="B101" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" t="s">
+        <v>41</v>
+      </c>
+      <c r="D101" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A102">
+        <v>833</v>
+      </c>
+      <c r="B102" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" t="s">
+        <v>7</v>
+      </c>
+      <c r="D102" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A103">
+        <v>834</v>
+      </c>
+      <c r="B103" t="s">
+        <v>80</v>
+      </c>
+      <c r="C103" t="s">
+        <v>7</v>
+      </c>
+      <c r="D103" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A104">
+        <v>835</v>
+      </c>
+      <c r="B104" t="s">
+        <v>80</v>
+      </c>
+      <c r="C104" t="s">
+        <v>7</v>
+      </c>
+      <c r="D104" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A105">
+        <v>836</v>
+      </c>
+      <c r="B105" t="s">
+        <v>80</v>
+      </c>
+      <c r="C105" t="s">
+        <v>7</v>
+      </c>
+      <c r="D105" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A106">
+        <v>844</v>
+      </c>
+      <c r="B106" t="s">
+        <v>81</v>
+      </c>
+      <c r="C106" t="s">
+        <v>82</v>
+      </c>
+      <c r="D106" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A107">
+        <v>845</v>
+      </c>
+      <c r="B107" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" t="s">
+        <v>41</v>
+      </c>
+      <c r="D107" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A108">
+        <v>846</v>
+      </c>
+      <c r="B108" t="s">
+        <v>43</v>
+      </c>
+      <c r="C108" t="s">
+        <v>5</v>
+      </c>
+      <c r="D108" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A109">
+        <v>847</v>
+      </c>
+      <c r="B109" t="s">
+        <v>43</v>
+      </c>
+      <c r="C109" t="s">
+        <v>5</v>
+      </c>
+      <c r="D109" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A110">
+        <v>851</v>
+      </c>
+      <c r="B110" t="s">
+        <v>7</v>
+      </c>
+      <c r="C110" t="s">
+        <v>84</v>
+      </c>
+      <c r="D110" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A111">
+        <v>852</v>
+      </c>
+      <c r="B111" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" t="s">
+        <v>41</v>
+      </c>
+      <c r="D111" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A112">
+        <v>855</v>
+      </c>
+      <c r="B112" t="s">
+        <v>80</v>
+      </c>
+      <c r="C112" t="s">
+        <v>7</v>
+      </c>
+      <c r="D112" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A113">
+        <v>856</v>
+      </c>
+      <c r="B113" t="s">
+        <v>43</v>
+      </c>
+      <c r="C113" t="s">
+        <v>5</v>
+      </c>
+      <c r="D113" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A114">
+        <v>858</v>
+      </c>
+      <c r="B114" t="s">
+        <v>7</v>
+      </c>
+      <c r="C114" t="s">
+        <v>84</v>
+      </c>
+      <c r="D114" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A115">
+        <v>859</v>
+      </c>
+      <c r="B115" t="s">
+        <v>43</v>
+      </c>
+      <c r="C115" t="s">
+        <v>7</v>
+      </c>
+      <c r="D115" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A116">
+        <v>864</v>
+      </c>
+      <c r="B116" t="s">
+        <v>48</v>
+      </c>
+      <c r="C116" t="s">
+        <v>49</v>
+      </c>
+      <c r="D116" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A117">
+        <v>871</v>
+      </c>
+      <c r="B117" t="s">
+        <v>5</v>
+      </c>
+      <c r="C117" t="s">
+        <v>39</v>
+      </c>
+      <c r="D117" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A118">
+        <v>885</v>
+      </c>
+      <c r="B118" t="s">
+        <v>14</v>
+      </c>
+      <c r="C118" t="s">
+        <v>17</v>
+      </c>
+      <c r="D118" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A119">
+        <v>888</v>
+      </c>
+      <c r="B119" t="s">
+        <v>14</v>
+      </c>
+      <c r="C119" t="s">
+        <v>17</v>
+      </c>
+      <c r="D119" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A120">
+        <v>889</v>
+      </c>
+      <c r="B120" t="s">
+        <v>4</v>
+      </c>
+      <c r="C120" t="s">
+        <v>10</v>
+      </c>
+      <c r="D120" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A121">
+        <v>890</v>
+      </c>
+      <c r="B121" t="s">
+        <v>4</v>
+      </c>
+      <c r="C121" t="s">
+        <v>10</v>
+      </c>
+      <c r="D121" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A122">
+        <v>891</v>
+      </c>
+      <c r="B122" t="s">
+        <v>4</v>
+      </c>
+      <c r="C122" t="s">
+        <v>10</v>
+      </c>
+      <c r="D122" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A123">
+        <v>893</v>
+      </c>
+      <c r="B123" t="s">
+        <v>14</v>
+      </c>
+      <c r="C123" t="s">
+        <v>87</v>
+      </c>
+      <c r="D123" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A124">
+        <v>894</v>
+      </c>
+      <c r="B124" t="s">
+        <v>4</v>
+      </c>
+      <c r="C124" t="s">
+        <v>10</v>
+      </c>
+      <c r="D124" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A125">
+        <v>897</v>
+      </c>
+      <c r="B125" t="s">
+        <v>41</v>
+      </c>
+      <c r="C125" t="s">
+        <v>88</v>
+      </c>
+      <c r="D125" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A126">
+        <v>898</v>
+      </c>
+      <c r="B126" t="s">
+        <v>43</v>
+      </c>
+      <c r="C126" t="s">
+        <v>90</v>
+      </c>
+      <c r="D126" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A127">
+        <v>901</v>
+      </c>
+      <c r="B127" t="s">
+        <v>80</v>
+      </c>
+      <c r="C127" t="s">
+        <v>7</v>
+      </c>
+      <c r="D127" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A128">
+        <v>903</v>
+      </c>
+      <c r="B128" t="s">
+        <v>43</v>
+      </c>
+      <c r="C128" t="s">
+        <v>5</v>
+      </c>
+      <c r="D128" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A129">
+        <v>917</v>
+      </c>
+      <c r="B129" t="s">
+        <v>7</v>
+      </c>
+      <c r="C129" t="s">
+        <v>41</v>
+      </c>
+      <c r="D129" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A130">
+        <v>921</v>
+      </c>
+      <c r="B130" t="s">
+        <v>43</v>
+      </c>
+      <c r="C130" t="s">
+        <v>5</v>
+      </c>
+      <c r="D130" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A131">
+        <v>922</v>
+      </c>
+      <c r="B131" t="s">
+        <v>43</v>
+      </c>
+      <c r="C131" t="s">
+        <v>5</v>
+      </c>
+      <c r="D131" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A132">
+        <v>923</v>
+      </c>
+      <c r="B132" t="s">
+        <v>43</v>
+      </c>
+      <c r="C132" t="s">
+        <v>5</v>
+      </c>
+      <c r="D132" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A133">
+        <v>924</v>
+      </c>
+      <c r="B133" t="s">
+        <v>5</v>
+      </c>
+      <c r="C133" t="s">
+        <v>41</v>
+      </c>
+      <c r="D133" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A134">
+        <v>925</v>
+      </c>
+      <c r="B134" t="s">
+        <v>43</v>
+      </c>
+      <c r="C134" t="s">
+        <v>5</v>
+      </c>
+      <c r="D134" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A135">
+        <v>926</v>
+      </c>
+      <c r="B135" t="s">
+        <v>92</v>
+      </c>
+      <c r="C135" t="s">
+        <v>41</v>
+      </c>
+      <c r="D135" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A136">
+        <v>928</v>
+      </c>
+      <c r="B136" t="s">
+        <v>48</v>
+      </c>
+      <c r="C136" t="s">
+        <v>10</v>
+      </c>
+      <c r="D136" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A137">
+        <v>929</v>
+      </c>
+      <c r="B137" t="s">
+        <v>92</v>
+      </c>
+      <c r="C137" t="s">
+        <v>94</v>
+      </c>
+      <c r="D137" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A138">
+        <v>932</v>
+      </c>
+      <c r="B138" t="s">
+        <v>24</v>
+      </c>
+      <c r="C138" t="s">
+        <v>58</v>
+      </c>
+      <c r="D138" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A139">
+        <v>939</v>
+      </c>
+      <c r="B139" t="s">
+        <v>96</v>
+      </c>
+      <c r="C139" t="s">
+        <v>97</v>
+      </c>
+      <c r="D139" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A140">
+        <v>940</v>
+      </c>
+      <c r="B140" t="s">
+        <v>46</v>
+      </c>
+      <c r="C140" t="s">
+        <v>98</v>
+      </c>
+      <c r="D140" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A141">
+        <v>941</v>
+      </c>
+      <c r="B141" t="s">
+        <v>46</v>
+      </c>
+      <c r="C141" t="s">
+        <v>58</v>
+      </c>
+      <c r="D141" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A142">
+        <v>956</v>
+      </c>
+      <c r="B142" t="s">
+        <v>6</v>
+      </c>
+      <c r="C142" t="s">
+        <v>24</v>
+      </c>
+      <c r="D142" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A143">
+        <v>968</v>
+      </c>
+      <c r="B143" t="s">
+        <v>48</v>
+      </c>
+      <c r="C143" t="s">
+        <v>49</v>
+      </c>
+      <c r="D143" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A144">
+        <v>971</v>
+      </c>
+      <c r="B144" t="s">
+        <v>48</v>
+      </c>
+      <c r="C144" t="s">
+        <v>49</v>
+      </c>
+      <c r="D144" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A145">
+        <v>972</v>
+      </c>
+      <c r="B145" t="s">
+        <v>48</v>
+      </c>
+      <c r="C145" t="s">
+        <v>49</v>
+      </c>
+      <c r="D145" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A146">
+        <v>984</v>
+      </c>
+      <c r="B146" t="s">
+        <v>14</v>
+      </c>
+      <c r="C146" t="s">
+        <v>17</v>
+      </c>
+      <c r="D146" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A147">
+        <v>987</v>
+      </c>
+      <c r="B147" t="s">
+        <v>14</v>
+      </c>
+      <c r="C147" t="s">
+        <v>17</v>
+      </c>
+      <c r="D147" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified and Annotated image 670 - 1000 (#14)
</commit_message>
<xml_diff>
--- a/Error_Annotations.xlsx
+++ b/Error_Annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spectroGUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC12CE6-52A8-4407-BAB9-55A4372B36FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178DEF00-58DB-4866-AA38-06FD30769D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="101">
   <si>
     <t>Picture Number</t>
   </si>
@@ -268,8 +268,23 @@
     <t>Alcohol, Alkene, Carboxylic Acids</t>
   </si>
   <si>
+    <t>Alcohol, Aldehyde, Amine</t>
+  </si>
+  <si>
+    <t>Alcohol, Aldehyde</t>
+  </si>
+  <si>
+    <t>Alcohol, Amine, Carboxylic Acids</t>
+  </si>
+  <si>
+    <t>Alcohol, Tertiary Amine, Carboxylic Acid</t>
+  </si>
+  <si>
+    <t>Nitrile, Alkene</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Alcohol, Symmertical / </t>
+      <t xml:space="preserve">Alcohol, Symmertrical / </t>
     </r>
     <r>
       <rPr>
@@ -294,23 +309,124 @@
     </r>
   </si>
   <si>
-    <t>Alcohol, Aldehyde, Amine</t>
-  </si>
-  <si>
-    <t>Alcohol, Aldehyde</t>
-  </si>
-  <si>
-    <t>Alcohol, Amine, Carboxylic Acids</t>
-  </si>
-  <si>
-    <t>Alcohol, Tertiary Amine, Carboxylic Acid</t>
+    <r>
+      <t xml:space="preserve">Nitrile, Symmertrical / </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Trans</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Alkene</t>
+    </r>
+  </si>
+  <si>
+    <t>Alkene, Ester</t>
+  </si>
+  <si>
+    <t>Narrow, strong peak at 1750 - 1730</t>
+  </si>
+  <si>
+    <t>Narrow, strong peak at 3300 - 3100</t>
+  </si>
+  <si>
+    <t>Nitrile</t>
+  </si>
+  <si>
+    <t>Nitrile, Amide</t>
+  </si>
+  <si>
+    <t>Nirtile, Alkene</t>
+  </si>
+  <si>
+    <t>Nitrile, Alkene, Amide</t>
+  </si>
+  <si>
+    <t>Narrow, strong peak at 3400, 3300, 3100</t>
+  </si>
+  <si>
+    <t>Aromatic, Alcohol, Phenol, Amine</t>
+  </si>
+  <si>
+    <t>Aromatic, Ketone</t>
+  </si>
+  <si>
+    <t>Aromatic, Ketone, Amine</t>
+  </si>
+  <si>
+    <t>Narrow, strong peak at 3400, 3200</t>
+  </si>
+  <si>
+    <t>Aromatic, Amine, Amide</t>
+  </si>
+  <si>
+    <t>Narrow, strong peak at 1680</t>
+  </si>
+  <si>
+    <t>No wide, strong peak at 3600 - 3100; Narrow strong peak at 3400, 3300</t>
+  </si>
+  <si>
+    <t>Alkene, Alcohol</t>
+  </si>
+  <si>
+    <t>Aromatic, Amide</t>
+  </si>
+  <si>
+    <t>Narrow, strong peak at 1680; Narrow strong peak at 3400, 3100</t>
+  </si>
+  <si>
+    <t>Aromatic, Alcohol, Phenol, Ketone</t>
+  </si>
+  <si>
+    <t>Narrow, strong peak at 1700</t>
+  </si>
+  <si>
+    <t>Aromatic, Alcohol, Carboxylic Acid</t>
+  </si>
+  <si>
+    <t>No narrow, strong peak at 1720</t>
+  </si>
+  <si>
+    <t>Aromatic, Carboxylic Acid</t>
+  </si>
+  <si>
+    <t>No wide, strong peak at 3600 - 3101</t>
+  </si>
+  <si>
+    <t>Alkene, Aldehyde</t>
+  </si>
+  <si>
+    <t>Alkene, Aldehyde, Alcohol</t>
+  </si>
+  <si>
+    <t>Ketone, Alcohol</t>
+  </si>
+  <si>
+    <t>No narrow, strong peak at 1650</t>
+  </si>
+  <si>
+    <t>No narrow, strong peak at 1700</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,19 +449,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -360,11 +476,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,16 +759,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B151" sqref="B151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.46484375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="61.46484375" bestFit="1" customWidth="1"/>
   </cols>
@@ -674,16 +788,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -702,16 +816,16 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="2">
+      <c r="A4">
         <v>45</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -730,58 +844,58 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="2">
+      <c r="A6">
         <v>71</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="2">
+      <c r="A7">
         <v>83</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="2">
+      <c r="A8">
         <v>84</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="2">
+      <c r="A9">
         <v>85</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>40</v>
       </c>
     </row>
@@ -800,16 +914,16 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" s="2">
+      <c r="A11">
         <v>113</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -856,198 +970,198 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" s="2">
+      <c r="A15">
         <v>153</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" s="2">
+      <c r="A16">
         <v>156</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" s="2">
+      <c r="A17">
         <v>157</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" s="2">
+      <c r="A18">
         <v>159</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="2">
+      <c r="A19">
         <v>175</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="2">
+      <c r="A20">
         <v>207</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" s="2">
+      <c r="A21">
         <v>208</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="2">
+      <c r="A22">
         <v>209</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" s="2">
+      <c r="A23">
         <v>210</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24" s="2">
+      <c r="A24">
         <v>212</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" s="2">
+      <c r="A25">
         <v>215</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" s="2">
+      <c r="A26">
         <v>221</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" s="2">
+      <c r="A27">
         <v>224</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A28" s="2">
+      <c r="A28">
         <v>272</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1080,16 +1194,16 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A31" s="2">
+      <c r="A31">
         <v>322</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1108,142 +1222,142 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A33" s="2">
+      <c r="A33">
         <v>336</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A34" s="2">
+      <c r="A34">
         <v>337</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A35" s="2">
+      <c r="A35">
         <v>339</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A36" s="2">
+      <c r="A36">
         <v>340</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A37" s="2">
+      <c r="A37">
         <v>341</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A38" s="2">
+      <c r="A38">
         <v>343</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="2" t="s">
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A39" s="2">
+      <c r="A39">
         <v>346</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A40" s="2">
+      <c r="A40">
         <v>347</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="2" t="s">
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
         <v>41</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A41" s="2">
+      <c r="A41">
         <v>348</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A42" s="2">
+      <c r="A42">
         <v>352</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1613,77 +1727,77 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69">
-        <v>510</v>
+        <v>533</v>
       </c>
       <c r="B69" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C69" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="D69" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70">
-        <v>533</v>
+        <v>553</v>
       </c>
       <c r="B70" t="s">
         <v>21</v>
       </c>
       <c r="C70" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="D70" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71">
-        <v>553</v>
+        <v>559</v>
       </c>
       <c r="B71" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C71" t="s">
-        <v>22</v>
-      </c>
-      <c r="D71" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D71" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B72" t="s">
         <v>18</v>
       </c>
       <c r="C72" t="s">
-        <v>27</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="D72" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B73" t="s">
         <v>18</v>
       </c>
       <c r="C73" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D73" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B74" t="s">
         <v>18</v>
@@ -1691,13 +1805,13 @@
       <c r="C74" t="s">
         <v>27</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="D74" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75">
-        <v>564</v>
+        <v>573</v>
       </c>
       <c r="B75" t="s">
         <v>18</v>
@@ -1705,75 +1819,75 @@
       <c r="C75" t="s">
         <v>27</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="D75" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76">
-        <v>573</v>
+        <v>580</v>
       </c>
       <c r="B76" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>27</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="D76" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77">
-        <v>580</v>
+        <v>616</v>
       </c>
       <c r="B77" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="C77" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="D77" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78">
-        <v>616</v>
+        <v>651</v>
       </c>
       <c r="B78" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="C78" t="s">
-        <v>66</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="D78" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B79" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="C79" t="s">
-        <v>19</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>20</v>
+        <v>68</v>
+      </c>
+      <c r="D79" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="B80" t="s">
+        <v>67</v>
+      </c>
+      <c r="C80" t="s">
         <v>68</v>
-      </c>
-      <c r="C80" t="s">
-        <v>69</v>
       </c>
       <c r="D80" t="s">
         <v>32</v>
@@ -1781,63 +1895,63 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B81" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="C81" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="D81" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="B82" t="s">
         <v>18</v>
       </c>
       <c r="C82" t="s">
-        <v>27</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="D82" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B83" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="C83" t="s">
-        <v>19</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>20</v>
+        <v>68</v>
+      </c>
+      <c r="D83" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84">
-        <v>661</v>
+        <v>666</v>
       </c>
       <c r="B84" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="C84" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="D84" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85">
-        <v>666</v>
+        <v>708</v>
       </c>
       <c r="B85" t="s">
         <v>18</v>
@@ -1845,11 +1959,880 @@
       <c r="C85" t="s">
         <v>19</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="D85" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A86">
+        <v>711</v>
+      </c>
+      <c r="B86" t="s">
+        <v>69</v>
+      </c>
+      <c r="C86" t="s">
+        <v>71</v>
+      </c>
+      <c r="D86" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A87">
+        <v>729</v>
+      </c>
+      <c r="B87" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87" t="s">
+        <v>72</v>
+      </c>
+      <c r="D87" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A88">
+        <v>730</v>
+      </c>
+      <c r="B88" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" t="s">
+        <v>72</v>
+      </c>
+      <c r="D88" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A89">
+        <v>736</v>
+      </c>
+      <c r="B89" t="s">
+        <v>6</v>
+      </c>
+      <c r="C89" t="s">
+        <v>37</v>
+      </c>
+      <c r="D89" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A90">
+        <v>739</v>
+      </c>
+      <c r="B90" t="s">
+        <v>75</v>
+      </c>
+      <c r="C90" t="s">
+        <v>76</v>
+      </c>
+      <c r="D90" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A91">
+        <v>750</v>
+      </c>
+      <c r="B91" t="s">
+        <v>77</v>
+      </c>
+      <c r="C91" t="s">
+        <v>71</v>
+      </c>
+      <c r="D91" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A92">
+        <v>751</v>
+      </c>
+      <c r="B92" t="s">
+        <v>77</v>
+      </c>
+      <c r="C92" t="s">
+        <v>78</v>
+      </c>
+      <c r="D92" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A93">
+        <v>785</v>
+      </c>
+      <c r="B93" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A94">
+        <v>786</v>
+      </c>
+      <c r="B94" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A95">
+        <v>788</v>
+      </c>
+      <c r="B95" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95" t="s">
+        <v>7</v>
+      </c>
+      <c r="D95" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A96">
+        <v>789</v>
+      </c>
+      <c r="B96" t="s">
+        <v>7</v>
+      </c>
+      <c r="C96" t="s">
+        <v>7</v>
+      </c>
+      <c r="D96" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A97">
+        <v>801</v>
+      </c>
+      <c r="B97" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A98">
+        <v>802</v>
+      </c>
+      <c r="B98" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" t="s">
+        <v>5</v>
+      </c>
+      <c r="D98" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A99">
+        <v>803</v>
+      </c>
+      <c r="B99" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99" t="s">
+        <v>41</v>
+      </c>
+      <c r="D99" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A100">
+        <v>804</v>
+      </c>
+      <c r="B100" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A101">
+        <v>811</v>
+      </c>
+      <c r="B101" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" t="s">
+        <v>41</v>
+      </c>
+      <c r="D101" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A102">
+        <v>833</v>
+      </c>
+      <c r="B102" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" t="s">
+        <v>7</v>
+      </c>
+      <c r="D102" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A103">
+        <v>834</v>
+      </c>
+      <c r="B103" t="s">
+        <v>80</v>
+      </c>
+      <c r="C103" t="s">
+        <v>7</v>
+      </c>
+      <c r="D103" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A104">
+        <v>835</v>
+      </c>
+      <c r="B104" t="s">
+        <v>80</v>
+      </c>
+      <c r="C104" t="s">
+        <v>7</v>
+      </c>
+      <c r="D104" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A105">
+        <v>836</v>
+      </c>
+      <c r="B105" t="s">
+        <v>80</v>
+      </c>
+      <c r="C105" t="s">
+        <v>7</v>
+      </c>
+      <c r="D105" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A106">
+        <v>844</v>
+      </c>
+      <c r="B106" t="s">
+        <v>81</v>
+      </c>
+      <c r="C106" t="s">
+        <v>82</v>
+      </c>
+      <c r="D106" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A107">
+        <v>845</v>
+      </c>
+      <c r="B107" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" t="s">
+        <v>41</v>
+      </c>
+      <c r="D107" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A108">
+        <v>846</v>
+      </c>
+      <c r="B108" t="s">
+        <v>43</v>
+      </c>
+      <c r="C108" t="s">
+        <v>5</v>
+      </c>
+      <c r="D108" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A109">
+        <v>847</v>
+      </c>
+      <c r="B109" t="s">
+        <v>43</v>
+      </c>
+      <c r="C109" t="s">
+        <v>5</v>
+      </c>
+      <c r="D109" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A110">
+        <v>851</v>
+      </c>
+      <c r="B110" t="s">
+        <v>7</v>
+      </c>
+      <c r="C110" t="s">
+        <v>84</v>
+      </c>
+      <c r="D110" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A111">
+        <v>852</v>
+      </c>
+      <c r="B111" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" t="s">
+        <v>41</v>
+      </c>
+      <c r="D111" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A112">
+        <v>855</v>
+      </c>
+      <c r="B112" t="s">
+        <v>80</v>
+      </c>
+      <c r="C112" t="s">
+        <v>7</v>
+      </c>
+      <c r="D112" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A113">
+        <v>856</v>
+      </c>
+      <c r="B113" t="s">
+        <v>43</v>
+      </c>
+      <c r="C113" t="s">
+        <v>5</v>
+      </c>
+      <c r="D113" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A114">
+        <v>858</v>
+      </c>
+      <c r="B114" t="s">
+        <v>7</v>
+      </c>
+      <c r="C114" t="s">
+        <v>84</v>
+      </c>
+      <c r="D114" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A115">
+        <v>859</v>
+      </c>
+      <c r="B115" t="s">
+        <v>43</v>
+      </c>
+      <c r="C115" t="s">
+        <v>7</v>
+      </c>
+      <c r="D115" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A116">
+        <v>864</v>
+      </c>
+      <c r="B116" t="s">
+        <v>48</v>
+      </c>
+      <c r="C116" t="s">
+        <v>49</v>
+      </c>
+      <c r="D116" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A117">
+        <v>871</v>
+      </c>
+      <c r="B117" t="s">
+        <v>5</v>
+      </c>
+      <c r="C117" t="s">
+        <v>39</v>
+      </c>
+      <c r="D117" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A118">
+        <v>885</v>
+      </c>
+      <c r="B118" t="s">
+        <v>14</v>
+      </c>
+      <c r="C118" t="s">
+        <v>17</v>
+      </c>
+      <c r="D118" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A119">
+        <v>888</v>
+      </c>
+      <c r="B119" t="s">
+        <v>14</v>
+      </c>
+      <c r="C119" t="s">
+        <v>17</v>
+      </c>
+      <c r="D119" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A120">
+        <v>889</v>
+      </c>
+      <c r="B120" t="s">
+        <v>4</v>
+      </c>
+      <c r="C120" t="s">
+        <v>10</v>
+      </c>
+      <c r="D120" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A121">
+        <v>890</v>
+      </c>
+      <c r="B121" t="s">
+        <v>4</v>
+      </c>
+      <c r="C121" t="s">
+        <v>10</v>
+      </c>
+      <c r="D121" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A122">
+        <v>891</v>
+      </c>
+      <c r="B122" t="s">
+        <v>4</v>
+      </c>
+      <c r="C122" t="s">
+        <v>10</v>
+      </c>
+      <c r="D122" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A123">
+        <v>893</v>
+      </c>
+      <c r="B123" t="s">
+        <v>14</v>
+      </c>
+      <c r="C123" t="s">
+        <v>87</v>
+      </c>
+      <c r="D123" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A124">
+        <v>894</v>
+      </c>
+      <c r="B124" t="s">
+        <v>4</v>
+      </c>
+      <c r="C124" t="s">
+        <v>10</v>
+      </c>
+      <c r="D124" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A125">
+        <v>897</v>
+      </c>
+      <c r="B125" t="s">
+        <v>41</v>
+      </c>
+      <c r="C125" t="s">
+        <v>88</v>
+      </c>
+      <c r="D125" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A126">
+        <v>898</v>
+      </c>
+      <c r="B126" t="s">
+        <v>43</v>
+      </c>
+      <c r="C126" t="s">
+        <v>90</v>
+      </c>
+      <c r="D126" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A127">
+        <v>901</v>
+      </c>
+      <c r="B127" t="s">
+        <v>80</v>
+      </c>
+      <c r="C127" t="s">
+        <v>7</v>
+      </c>
+      <c r="D127" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A128">
+        <v>903</v>
+      </c>
+      <c r="B128" t="s">
+        <v>43</v>
+      </c>
+      <c r="C128" t="s">
+        <v>5</v>
+      </c>
+      <c r="D128" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A129">
+        <v>917</v>
+      </c>
+      <c r="B129" t="s">
+        <v>7</v>
+      </c>
+      <c r="C129" t="s">
+        <v>41</v>
+      </c>
+      <c r="D129" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A130">
+        <v>921</v>
+      </c>
+      <c r="B130" t="s">
+        <v>43</v>
+      </c>
+      <c r="C130" t="s">
+        <v>5</v>
+      </c>
+      <c r="D130" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A131">
+        <v>922</v>
+      </c>
+      <c r="B131" t="s">
+        <v>43</v>
+      </c>
+      <c r="C131" t="s">
+        <v>5</v>
+      </c>
+      <c r="D131" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A132">
+        <v>923</v>
+      </c>
+      <c r="B132" t="s">
+        <v>43</v>
+      </c>
+      <c r="C132" t="s">
+        <v>5</v>
+      </c>
+      <c r="D132" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A133">
+        <v>924</v>
+      </c>
+      <c r="B133" t="s">
+        <v>5</v>
+      </c>
+      <c r="C133" t="s">
+        <v>41</v>
+      </c>
+      <c r="D133" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A134">
+        <v>925</v>
+      </c>
+      <c r="B134" t="s">
+        <v>43</v>
+      </c>
+      <c r="C134" t="s">
+        <v>5</v>
+      </c>
+      <c r="D134" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A135">
+        <v>926</v>
+      </c>
+      <c r="B135" t="s">
+        <v>92</v>
+      </c>
+      <c r="C135" t="s">
+        <v>41</v>
+      </c>
+      <c r="D135" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A136">
+        <v>928</v>
+      </c>
+      <c r="B136" t="s">
+        <v>48</v>
+      </c>
+      <c r="C136" t="s">
+        <v>10</v>
+      </c>
+      <c r="D136" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A137">
+        <v>929</v>
+      </c>
+      <c r="B137" t="s">
+        <v>92</v>
+      </c>
+      <c r="C137" t="s">
+        <v>94</v>
+      </c>
+      <c r="D137" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A138">
+        <v>932</v>
+      </c>
+      <c r="B138" t="s">
+        <v>24</v>
+      </c>
+      <c r="C138" t="s">
+        <v>58</v>
+      </c>
+      <c r="D138" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A139">
+        <v>939</v>
+      </c>
+      <c r="B139" t="s">
+        <v>96</v>
+      </c>
+      <c r="C139" t="s">
+        <v>97</v>
+      </c>
+      <c r="D139" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A140">
+        <v>940</v>
+      </c>
+      <c r="B140" t="s">
+        <v>46</v>
+      </c>
+      <c r="C140" t="s">
+        <v>98</v>
+      </c>
+      <c r="D140" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A141">
+        <v>941</v>
+      </c>
+      <c r="B141" t="s">
+        <v>46</v>
+      </c>
+      <c r="C141" t="s">
+        <v>58</v>
+      </c>
+      <c r="D141" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A142">
+        <v>956</v>
+      </c>
+      <c r="B142" t="s">
+        <v>6</v>
+      </c>
+      <c r="C142" t="s">
+        <v>24</v>
+      </c>
+      <c r="D142" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A143">
+        <v>968</v>
+      </c>
+      <c r="B143" t="s">
+        <v>48</v>
+      </c>
+      <c r="C143" t="s">
+        <v>49</v>
+      </c>
+      <c r="D143" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A144">
+        <v>971</v>
+      </c>
+      <c r="B144" t="s">
+        <v>48</v>
+      </c>
+      <c r="C144" t="s">
+        <v>49</v>
+      </c>
+      <c r="D144" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A145">
+        <v>972</v>
+      </c>
+      <c r="B145" t="s">
+        <v>48</v>
+      </c>
+      <c r="C145" t="s">
+        <v>49</v>
+      </c>
+      <c r="D145" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A146">
+        <v>984</v>
+      </c>
+      <c r="B146" t="s">
+        <v>14</v>
+      </c>
+      <c r="C146" t="s">
+        <v>17</v>
+      </c>
+      <c r="D146" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A147">
+        <v>987</v>
+      </c>
+      <c r="B147" t="s">
+        <v>14</v>
+      </c>
+      <c r="C147" t="s">
+        <v>17</v>
+      </c>
+      <c r="D147" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>